<commit_message>
Added Clinical Trial Templates
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/Basic Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/Basic Templates.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="27030" windowHeight="9885" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="585" windowWidth="27030" windowHeight="9885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
     <sheet name="CT" sheetId="2" r:id="rId2"/>
     <sheet name="Palliative" sheetId="3" r:id="rId3"/>
     <sheet name="Extremity" sheetId="4" r:id="rId4"/>
+    <sheet name="Basic Test" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="109">
   <si>
     <t>Reviewed</t>
   </si>
@@ -341,6 +342,12 @@
   </si>
   <si>
     <t>TemplateFileName</t>
+  </si>
+  <si>
+    <t>BasicTest</t>
+  </si>
+  <si>
+    <t>z Ring</t>
   </si>
 </sst>
 </file>
@@ -745,7 +752,258 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1596,7 +1854,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table35697142" displayName="Table35697142" ref="A2:B13" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table35697142" displayName="Table35697142" ref="A2:B13" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -1605,22 +1863,37 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table570724511" displayName="Table570724511" ref="D2:G8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <sortState ref="D3:H61">
+    <sortCondition ref="E3:E61"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Structure" dataDxfId="3"/>
+    <tableColumn id="2" name="ID" dataDxfId="2"/>
+    <tableColumn id="4" name="Name" dataDxfId="1"/>
+    <tableColumn id="3" name="ColorAndStyle" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5707245" displayName="Table5707245" ref="D2:F8" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5707245" displayName="Table5707245" ref="D2:F8" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49" totalsRowBorderDxfId="48">
   <sortState ref="D3:H61">
     <sortCondition ref="E3:E61"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="35"/>
-    <tableColumn id="2" name="ID" dataDxfId="34"/>
-    <tableColumn id="3" name="Name" dataDxfId="33"/>
+    <tableColumn id="1" name="Structure" dataDxfId="47"/>
+    <tableColumn id="2" name="ID" dataDxfId="46"/>
+    <tableColumn id="3" name="Name" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table35697173" displayName="Table35697173" ref="A2:B13" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table35697173" displayName="Table35697173" ref="A2:B13" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -1630,21 +1903,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5707274" displayName="Table5707274" ref="D2:F4" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5707274" displayName="Table5707274" ref="D2:F4" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <sortState ref="D3:H61">
     <sortCondition ref="E3:E61"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="24"/>
-    <tableColumn id="2" name="ID" dataDxfId="23"/>
-    <tableColumn id="3" name="Name" dataDxfId="22"/>
+    <tableColumn id="1" name="Structure" dataDxfId="36"/>
+    <tableColumn id="2" name="ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Name" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356971" displayName="Table356971" ref="A2:B13" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table356971" displayName="Table356971" ref="A2:B13" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -1654,21 +1927,21 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57072" displayName="Table57072" ref="D2:F19" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57072" displayName="Table57072" ref="D2:F19" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <sortState ref="D3:H61">
     <sortCondition ref="E3:E61"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="13"/>
-    <tableColumn id="2" name="ID" dataDxfId="12"/>
-    <tableColumn id="3" name="Name" dataDxfId="11"/>
+    <tableColumn id="1" name="Structure" dataDxfId="25"/>
+    <tableColumn id="2" name="ID" dataDxfId="24"/>
+    <tableColumn id="3" name="Name" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table33132343155" displayName="Table33132343155" ref="A2:B13" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table33132343155" displayName="Table33132343155" ref="A2:B13" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <tableColumns count="2">
     <tableColumn id="1" name="Attribute"/>
     <tableColumn id="2" name="Value"/>
@@ -1678,13 +1951,23 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table533353756" displayName="Table533353756" ref="D2:F16" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table533353756" displayName="Table533353756" ref="D2:F16" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <tableColumns count="3">
-    <tableColumn id="1" name="Structure" dataDxfId="2"/>
-    <tableColumn id="2" name="ID" dataDxfId="1"/>
-    <tableColumn id="3" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" name="Structure" dataDxfId="14"/>
+    <tableColumn id="2" name="ID" dataDxfId="13"/>
+    <tableColumn id="3" name="Name" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table3569714210" displayName="Table3569714210" ref="A2:B13" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Attribute"/>
+    <tableColumn id="2" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4096,7 +4379,7 @@
   </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B22:B23"/>
     </sheetView>
   </sheetViews>
@@ -5128,4 +5411,592 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="I1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="39"/>
+      <c r="O1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="37"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="22" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Body</v>
+      </c>
+      <c r="J3" s="21" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="K3" s="21" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="L3" s="20" t="str">
+        <f>VLOOKUP(D3,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="M3" s="19" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="N3" s="18" t="str">
+        <f>VLOOKUP(D3,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>BODY</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q3" s="16" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R3" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="15">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v>-350</v>
+      </c>
+      <c r="T3" s="14">
+        <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="22" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Treated Volume</v>
+      </c>
+      <c r="J4" s="21" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>Treated Volume</v>
+      </c>
+      <c r="K4" s="21" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="L4" s="20" t="str">
+        <f>VLOOKUP(D4,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="M4" s="19" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Special</v>
+      </c>
+      <c r="N4" s="18" t="str">
+        <f>VLOOKUP(D4,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P4" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q4" s="16" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S4" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T4" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="22" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>GTV Primary</v>
+      </c>
+      <c r="J5" s="21" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>GTVp</v>
+      </c>
+      <c r="K5" s="21" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="L5" s="20" t="str">
+        <f>VLOOKUP(D5,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="M5" s="19" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="N5" s="18" t="str">
+        <f>VLOOKUP(D5,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>GTV</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P5" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="16" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S5" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T5" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="22" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>CTV Primary</v>
+      </c>
+      <c r="J6" s="21" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>CTVp</v>
+      </c>
+      <c r="K6" s="21" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="L6" s="20" t="str">
+        <f>VLOOKUP(D6,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="M6" s="19" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="N6" s="18" t="str">
+        <f>VLOOKUP(D6,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>CTV</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P6" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q6" s="16" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S6" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T6" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="22" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>PTV Primary</v>
+      </c>
+      <c r="J7" s="21" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>PTVp</v>
+      </c>
+      <c r="K7" s="21" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>99VMS_STRUCTCODE</v>
+      </c>
+      <c r="L7" s="20" t="str">
+        <f>VLOOKUP(D7,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>1.0</v>
+      </c>
+      <c r="M7" s="19" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="N7" s="18" t="str">
+        <f>VLOOKUP(D7,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>PTV</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q7" s="16" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S7" s="15" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T7" s="14" t="str">
+        <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],3,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="J8" s="9">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],4,FALSE)</f>
+        <v>11296</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],5,FALSE)</f>
+        <v>RADLEX</v>
+      </c>
+      <c r="L8" s="8">
+        <f>VLOOKUP(D8,[1]!Dictionary[#All],6,FALSE)</f>
+        <v>3.8</v>
+      </c>
+      <c r="M8" s="7" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],2,FALSE)</f>
+        <v>Artifact</v>
+      </c>
+      <c r="N8" s="6" t="str">
+        <f>VLOOKUP(D8,[1]!VolumeType[#All],3,FALSE)</f>
+        <v>None</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="P8" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="R8" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="3" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="T8" s="2" t="str">
+        <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:R1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prostate Notes and Kidney code
Changed structure ID for iliac nodes in prostate and fixed FMA code for kidneys B
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/Basic Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/Basic Templates.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="585" windowWidth="27030" windowHeight="9885" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="585" windowWidth="27030" windowHeight="9885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
@@ -1835,6 +1835,7 @@
       <sheetName val="ICD-10 Codes"/>
       <sheetName val="Color Chart"/>
       <sheetName val="Original Structure colors"/>
+      <sheetName val="ColourTable"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -1848,6 +1849,7 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3175,7 +3177,7 @@
   </sheetPr>
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
@@ -4130,11 +4132,11 @@
       </c>
       <c r="H16" s="22" t="str">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],3,FALSE)</f>
-        <v>Kidney</v>
-      </c>
-      <c r="I16" s="21">
+        <v>Set of kidneys</v>
+      </c>
+      <c r="I16" s="21" t="str">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],4,FALSE)</f>
-        <v>7203</v>
+        <v>264815</v>
       </c>
       <c r="J16" s="21" t="str">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],5,FALSE)</f>
@@ -5420,7 +5422,7 @@
   </sheetPr>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>